<commit_message>
1. Main Scene bounds checking
</commit_message>
<xml_diff>
--- a/Reports/Work Load/Task List Report 1 - Preview and Review(Week 1).xlsx
+++ b/Reports/Work Load/Task List Report 1 - Preview and Review(Week 1).xlsx
@@ -16,13 +16,13 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E11">
+    <comment authorId="0" ref="E10">
       <text>
         <t xml:space="preserve">HONG CHRIS:
 Estimated volume of the task</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L11">
+    <comment authorId="0" ref="L10">
       <text>
         <t xml:space="preserve">HONG CHRIS:
 Actual volume after work done</t>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Task List Report 1 - Preview / Review (Week 1)</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>From</t>
-  </si>
-  <si>
-    <t>Lim ZiYi Jean</t>
-  </si>
-  <si>
-    <t>M2</t>
   </si>
   <si>
     <t>Shishanth Kaliannan</t>
@@ -144,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">Character Movement </t>
+  </si>
+  <si>
+    <t>M2</t>
   </si>
   <si>
     <t>Put in limits as to how the character will be able to move</t>
@@ -794,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="99">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -839,9 +836,6 @@
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="3" fillId="3" fontId="4" numFmtId="15" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -851,25 +845,13 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="9" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -955,6 +937,9 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -986,6 +971,9 @@
     </xf>
     <xf borderId="32" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1156,18 +1144,17 @@
       <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="str">
-        <f>SUMIF(D$12:D29, D4, E$12:E29)</f>
-        <v>8</v>
+      <c r="E4" s="17">
+        <v>12.0</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>18.0</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>42779.0</v>
       </c>
       <c r="J4" s="14"/>
@@ -1178,24 +1165,27 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="22" t="str">
-        <f>SUMIF(D$12:D29, D5, E$12:E29)</f>
-        <v>16</v>
+      <c r="E5" s="22">
+        <v>18.0</v>
       </c>
-      <c r="F5" s="23">
-        <v>19.0</v>
+      <c r="F5" s="22">
+        <v>20.0</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="19"/>
+      <c r="H5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="18">
+        <v>42797.0</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -1204,27 +1194,26 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="24" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25" t="str">
-        <f>SUMIF(D$11:D28, D6, E$11:E28)</f>
+      <c r="D6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="26">
-        <v>20.0</v>
+      <c r="E6" s="24">
+        <v>13.0</v>
+      </c>
+      <c r="F6" s="24">
+        <v>11.0</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
-      <c r="I6" s="19">
-        <v>42797.0</v>
+      <c r="I6" s="25">
+        <v>42779.0</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5"/>
@@ -1234,27 +1223,18 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="28" t="str">
-        <f>SUMIF(D$12:D30, D7, E$12:E30)</f>
-        <v>9</v>
-      </c>
-      <c r="F7" s="29">
-        <v>11.0</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="30">
-        <v>42779.0</v>
+      <c r="I7" s="28">
+        <v>42786.0</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="5"/>
@@ -1264,20 +1244,16 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="33">
-        <v>42786.0</v>
-      </c>
-      <c r="J8" s="14"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
@@ -1285,725 +1261,725 @@
       <c r="O8" s="5"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="34" t="s">
+      <c r="A9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37" t="s">
+      <c r="K9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="40" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="E10" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43" t="s">
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="43" t="s">
-        <v>2</v>
+      <c r="L10" s="44" t="s">
+        <v>3</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="M10" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48" t="s">
+      <c r="N10" s="30"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="46">
+        <v>1.0</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="M11" s="50" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="35"/>
-      <c r="O11" s="39"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="51">
-        <v>1.0</v>
+      <c r="E11" s="17">
+        <v>2.0</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54" t="s">
+      <c r="K11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="18">
+      <c r="L11" s="17">
         <v>2.0</v>
       </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="57" t="s">
+      <c r="M11" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="N11" s="55"/>
+      <c r="O11" s="56"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="57">
+        <v>2.0</v>
+      </c>
+      <c r="B12" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="18">
+      <c r="C12" s="8"/>
+      <c r="D12" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="59">
+        <v>4.0</v>
+      </c>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="59">
+        <v>5.0</v>
+      </c>
+      <c r="M12" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="61"/>
+      <c r="O12" s="63"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="57">
+        <v>3.0</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="59">
         <v>2.0</v>
       </c>
-      <c r="M12" s="59" t="s">
-        <v>30</v>
+      <c r="F13" s="64"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="62" t="s">
+        <v>33</v>
       </c>
-      <c r="N12" s="60"/>
-      <c r="O12" s="61"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="62">
+      <c r="K13" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="59">
         <v>2.0</v>
       </c>
-      <c r="B13" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="23">
+      <c r="M13" s="66"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="63"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="57">
         <v>4.0</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="23">
-        <v>5.0</v>
-      </c>
-      <c r="M13" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="65"/>
-      <c r="O13" s="67"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="62">
-        <v>3.0</v>
-      </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="58" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="59">
+        <v>2.0</v>
+      </c>
+      <c r="F14" s="64"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="59">
+        <v>2.0</v>
+      </c>
+      <c r="M14" s="66"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="63"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="65">
+        <v>5.0</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="59">
+        <v>3.0</v>
+      </c>
+      <c r="F15" s="64"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="59">
+        <v>3.0</v>
+      </c>
+      <c r="M15" s="66"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="63"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="65">
+        <v>6.0</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="59">
+        <v>2.0</v>
+      </c>
+      <c r="F16" s="64"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="59">
+        <v>2.0</v>
+      </c>
+      <c r="M16" s="66"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="63"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="65">
+        <v>7.0</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="59">
+        <v>4.0</v>
+      </c>
+      <c r="F17" s="60"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="23">
+      <c r="L17" s="59">
+        <v>6.0</v>
+      </c>
+      <c r="M17" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="61"/>
+      <c r="O17" s="63"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="65">
+        <v>8.0</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="59">
         <v>2.0</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="66" t="s">
+      <c r="F18" s="60"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="59">
+        <v>2.0</v>
+      </c>
+      <c r="M18" s="66"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="63"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="65">
+        <v>9.0</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="L14" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="M14" s="70"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="67"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="62">
+      <c r="E19" s="59">
         <v>4.0</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>36</v>
+      <c r="F19" s="64"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="67" t="s">
+        <v>47</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="23" t="s">
+      <c r="K19" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="59">
+        <v>4.0</v>
+      </c>
+      <c r="M19" s="66"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="63"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="65">
+        <v>10.0</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="23">
-        <v>2.0</v>
+      <c r="E20" s="59">
+        <v>6.0</v>
       </c>
-      <c r="F15" s="68"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="66" t="s">
-        <v>37</v>
+      <c r="F20" s="64"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="67" t="s">
+        <v>49</v>
       </c>
-      <c r="K15" s="69" t="s">
+      <c r="K20" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="23">
-        <v>2.0</v>
+      <c r="L20" s="59">
+        <v>8.0</v>
       </c>
-      <c r="M15" s="70"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="67"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="69">
-        <v>5.0</v>
+      <c r="M20" s="64" t="s">
+        <v>50</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>38</v>
+      <c r="N20" s="61"/>
+      <c r="O20" s="63"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="65">
+        <v>11.0</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="23" t="s">
-        <v>11</v>
+      <c r="B21" s="58" t="s">
+        <v>51</v>
       </c>
-      <c r="E16" s="23">
+      <c r="C21" s="8"/>
+      <c r="D21" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="59">
         <v>3.0</v>
       </c>
-      <c r="F16" s="68"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="58" t="s">
-        <v>39</v>
+      <c r="F21" s="60"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="70" t="s">
+        <v>52</v>
       </c>
-      <c r="K16" s="69" t="s">
-        <v>11</v>
+      <c r="K21" s="68" t="s">
+        <v>14</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L21" s="59">
         <v>3.0</v>
       </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="67"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="69">
-        <v>6.0</v>
+      <c r="M21" s="66"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="63"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="65">
+        <v>12.0</v>
       </c>
-      <c r="B17" s="63" t="s">
-        <v>40</v>
+      <c r="B22" s="58" t="s">
+        <v>53</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="54" t="s">
-        <v>27</v>
+      <c r="C22" s="8"/>
+      <c r="D22" s="59" t="s">
+        <v>14</v>
       </c>
-      <c r="E17" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="F17" s="68"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="M17" s="70"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="67"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="69">
-        <v>7.0</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="23">
+      <c r="E22" s="59">
         <v>4.0</v>
       </c>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="71" t="s">
-        <v>43</v>
+      <c r="F22" s="66"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="65" t="s">
+        <v>14</v>
       </c>
-      <c r="K18" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="L18" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="M18" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" s="65"/>
-      <c r="O18" s="67"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="69">
-        <v>8.0</v>
-      </c>
-      <c r="B19" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="M19" s="70"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="67"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="69">
-        <v>9.0</v>
-      </c>
-      <c r="B20" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="23">
+      <c r="L22" s="59">
         <v>4.0</v>
       </c>
-      <c r="F20" s="68"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="71" t="s">
-        <v>48</v>
+      <c r="M22" s="66"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="63"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="65">
+        <v>13.0</v>
       </c>
-      <c r="K20" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="23">
-        <v>4.0</v>
-      </c>
-      <c r="M20" s="70"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="67"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="69">
-        <v>10.0</v>
-      </c>
-      <c r="B21" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="F21" s="68"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="23">
-        <v>8.0</v>
-      </c>
-      <c r="M21" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="N21" s="65"/>
-      <c r="O21" s="67"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="69">
-        <v>11.0</v>
-      </c>
-      <c r="B22" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="L22" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="M22" s="70"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="67"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="69">
-        <v>12.0</v>
-      </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="58" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="23" t="s">
-        <v>16</v>
+      <c r="D23" s="59" t="s">
+        <v>11</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="59">
         <v>4.0</v>
       </c>
-      <c r="F23" s="70"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="L23" s="23">
-        <v>4.0</v>
-      </c>
-      <c r="M23" s="70"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="67"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="69">
-        <v>13.0</v>
-      </c>
-      <c r="B24" s="63" t="s">
+      <c r="J23" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="23" t="s">
-        <v>13</v>
+      <c r="K23" s="65" t="s">
+        <v>11</v>
       </c>
-      <c r="E24" s="23">
-        <v>4.0</v>
+      <c r="L23" s="59">
+        <v>3.0</v>
       </c>
-      <c r="F24" s="68"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="58" t="s">
+      <c r="M23" s="66"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="63"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="65">
+        <v>14.0</v>
+      </c>
+      <c r="B24" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="69" t="s">
-        <v>13</v>
+      <c r="C24" s="8"/>
+      <c r="D24" s="59" t="s">
+        <v>8</v>
       </c>
-      <c r="L24" s="23">
-        <v>3.0</v>
+      <c r="E24" s="59">
+        <v>6.0</v>
       </c>
-      <c r="M24" s="70"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="67"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="59">
+        <v>6.0</v>
+      </c>
+      <c r="M24" s="66"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="63"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="69">
-        <v>14.0</v>
+      <c r="A25" s="65">
+        <v>15.0</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="58" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="23" t="s">
-        <v>8</v>
+      <c r="D25" s="59" t="s">
+        <v>35</v>
       </c>
-      <c r="E25" s="23">
-        <v>6.0</v>
+      <c r="E25" s="59">
+        <v>3.0</v>
       </c>
-      <c r="F25" s="70"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" s="23">
-        <v>6.0</v>
-      </c>
-      <c r="M25" s="70"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="67"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="69">
-        <v>15.0</v>
-      </c>
-      <c r="B26" s="63" t="s">
+      <c r="J25" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="23" t="s">
-        <v>11</v>
+      <c r="K25" s="65" t="s">
+        <v>35</v>
       </c>
-      <c r="E26" s="23">
+      <c r="L25" s="59">
         <v>3.0</v>
       </c>
-      <c r="F26" s="68"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="63"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="65">
+        <v>16.0</v>
+      </c>
+      <c r="B26" s="72"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="73" t="s">
+      <c r="J26" s="71"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="63"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="65">
+        <v>17.0</v>
+      </c>
+      <c r="B27" s="72"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="63"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="65">
+        <v>18.0</v>
+      </c>
+      <c r="B28" s="72"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="63"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="K26" s="69" t="s">
-        <v>11</v>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77" t="str">
+        <f>SUM(E11:E28)</f>
+        <v>51</v>
       </c>
-      <c r="L26" s="23">
-        <v>3.0</v>
+      <c r="F29" s="78"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="77" t="str">
+        <f>SUM(L11:L28)</f>
+        <v>55</v>
       </c>
-      <c r="M26" s="70"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="67"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="69">
-        <v>16.0</v>
-      </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="67"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="69">
-        <v>17.0</v>
-      </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="67"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="69">
-        <v>18.0</v>
-      </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="67"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="81"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="79"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80" t="str">
-        <f>SUM(E12:E29)</f>
-        <v>51</v>
+      <c r="B31" s="61"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="82" t="s">
+        <v>61</v>
       </c>
-      <c r="F30" s="81"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="80" t="str">
-        <f>SUM(L12:L29)</f>
-        <v>55</v>
-      </c>
-      <c r="M30" s="81"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="84"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="5"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="83"/>
+      <c r="O31" s="84"/>
+      <c r="P31" s="14"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="85" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="88"/>
       <c r="K32" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="L32" s="65"/>
-      <c r="M32" s="8"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
       <c r="N32" s="86"/>
       <c r="O32" s="87"/>
-      <c r="P32" s="14"/>
+      <c r="P32" s="89"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="88" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="88" t="s">
-        <v>63</v>
-      </c>
-      <c r="L33" s="89"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="89"/>
-      <c r="O33" s="90"/>
-      <c r="P33" s="92"/>
+      <c r="A33" s="90"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="90"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="89"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="93"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="93"/>
-      <c r="O34" s="94"/>
-      <c r="P34" s="92"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="88"/>
+      <c r="K34" s="92"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="48"/>
+      <c r="P34" s="89"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="95"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="91"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="92"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4"/>
@@ -2023,143 +1999,143 @@
       <c r="O36" s="5"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="5"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="95"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="96"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="99" t="str">
+      <c r="A38" s="96" t="str">
         <f>C4</f>
         <v>Lucas Nguyen Thai Vinh</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="100" t="str">
-        <f>C5</f>
-        <v>Lim ZiYi Jean</v>
+      <c r="D38" s="4"/>
+      <c r="E38" s="97" t="str">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
-      <c r="F39" s="89"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="100" t="str">
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="97" t="str">
         <f>C4</f>
         <v>Lucas Nguyen Thai Vinh</v>
       </c>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="101" t="str">
-        <f>C5</f>
-        <v>Lim ZiYi Jean</v>
-      </c>
-      <c r="P39" s="14"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-    </row>
-    <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="96"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="97"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="98"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-    </row>
-    <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="99" t="str">
+      <c r="L38" s="86"/>
+      <c r="M38" s="86"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="98" t="str">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="100" t="str">
-        <f>C8</f>
-        <v/>
-      </c>
-      <c r="F42" s="89"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="89"/>
-      <c r="J42" s="99"/>
-      <c r="K42" s="100" t="str">
+      <c r="P38" s="14"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" ht="12.75" customHeight="1">
+      <c r="A40" s="93"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="95"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+    </row>
+    <row r="41" ht="12.75" customHeight="1">
+      <c r="A41" s="96" t="str">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L42" s="89"/>
-      <c r="M42" s="89"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="101" t="str">
-        <f>C8</f>
+      <c r="D41" s="4"/>
+      <c r="E41" s="97" t="str">
+        <f>C7</f>
         <v/>
       </c>
-      <c r="P42" s="14"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="86"/>
+      <c r="I41" s="86"/>
+      <c r="J41" s="96"/>
+      <c r="K41" s="97" t="str">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L41" s="86"/>
+      <c r="M41" s="86"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="98" t="str">
+        <f>C7</f>
+        <v/>
+      </c>
+      <c r="P41" s="14"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="5"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="6"/>
@@ -18435,104 +18411,87 @@
       <c r="N1000" s="6"/>
       <c r="O1000" s="5"/>
     </row>
-    <row r="1001" ht="15.75" customHeight="1">
-      <c r="A1001" s="5"/>
-      <c r="B1001" s="5"/>
-      <c r="C1001" s="5"/>
-      <c r="D1001" s="5"/>
-      <c r="E1001" s="5"/>
-      <c r="F1001" s="5"/>
-      <c r="G1001" s="6"/>
-      <c r="H1001" s="6"/>
-      <c r="I1001" s="6"/>
-      <c r="J1001" s="6"/>
-      <c r="K1001" s="5"/>
-      <c r="L1001" s="5"/>
-      <c r="M1001" s="6"/>
-      <c r="N1001" s="6"/>
-      <c r="O1001" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F25:I25"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A32:I34"/>
+    <mergeCell ref="K32:O34"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="F26:I26"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A33:I35"/>
-    <mergeCell ref="K33:O35"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A32:C32"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M25:O25"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="M14:O14"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K9:O9"/>
+    <mergeCell ref="M11:O11"/>
     <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="E37:I37"/>
     <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="F21:I21"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:I20"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M21:O21"/>
     <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M22:O22"/>
     <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M26:O26"/>
     <mergeCell ref="M27:O27"/>
     <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>